<commit_message>
Added new swords, and worked on item generation/inventory bugs
</commit_message>
<xml_diff>
--- a/Rougelike Game/ItemLevels.xlsx
+++ b/Rougelike Game/ItemLevels.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA17A3BE-0144-4D68-97A8-96B4547C1889}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A338F2-C050-46D6-9DD4-51B7C9F60FC0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="82">
   <si>
     <t>Leather</t>
   </si>
@@ -167,6 +167,105 @@
   </si>
   <si>
     <t>ruby</t>
+  </si>
+  <si>
+    <t>Icicle</t>
+  </si>
+  <si>
+    <t>Bone Sword</t>
+  </si>
+  <si>
+    <t>Obsidian Blade</t>
+  </si>
+  <si>
+    <t>Claymore</t>
+  </si>
+  <si>
+    <t>Weed Whacker</t>
+  </si>
+  <si>
+    <t>Mist Saber</t>
+  </si>
+  <si>
+    <t>Magma Blade</t>
+  </si>
+  <si>
+    <t>Lightsaber</t>
+  </si>
+  <si>
+    <t>Golden Khopesh</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t>Templar sword</t>
+  </si>
+  <si>
+    <t>Destroyer</t>
+  </si>
+  <si>
+    <t>Wooden Shaft</t>
+  </si>
+  <si>
+    <t>Treasure Blade</t>
+  </si>
+  <si>
+    <t>Ruby Blade</t>
+  </si>
+  <si>
+    <t>Dragonbone Blade</t>
+  </si>
+  <si>
+    <t>Elven Sword</t>
+  </si>
+  <si>
+    <t>Serpent Sword</t>
+  </si>
+  <si>
+    <t>Amethyst Shaft</t>
+  </si>
+  <si>
+    <t>Captain's Sword</t>
+  </si>
+  <si>
+    <t>Bronze Destroyer</t>
+  </si>
+  <si>
+    <t>Iron Khopesh</t>
+  </si>
+  <si>
+    <t>Opal</t>
+  </si>
+  <si>
+    <t>Cleaver</t>
+  </si>
+  <si>
+    <t>Magic Sword</t>
+  </si>
+  <si>
+    <t>Ceremony Sword</t>
+  </si>
+  <si>
+    <t>Relic Sword</t>
+  </si>
+  <si>
+    <t>Eversteel Sword</t>
+  </si>
+  <si>
+    <t>Jeweled sword</t>
+  </si>
+  <si>
+    <t>Rhrodochrosite Blade</t>
+  </si>
+  <si>
+    <t>Coral Sword</t>
+  </si>
+  <si>
+    <t>Quartz Sword</t>
   </si>
 </sst>
 </file>
@@ -484,15 +583,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,8 +604,14 @@
       <c r="F1">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -519,8 +624,14 @@
       <c r="F2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -533,8 +644,14 @@
       <c r="F3">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -547,8 +664,14 @@
       <c r="F4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -561,8 +684,14 @@
       <c r="F5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -575,8 +704,14 @@
       <c r="F6">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -589,8 +724,14 @@
       <c r="F7">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -603,8 +744,14 @@
       <c r="F8">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -617,8 +764,14 @@
       <c r="F9">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -631,8 +784,14 @@
       <c r="F10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -645,8 +804,14 @@
       <c r="F11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -659,8 +824,14 @@
       <c r="F12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -673,8 +844,14 @@
       <c r="F13">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -687,8 +864,14 @@
       <c r="F14">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -701,8 +884,14 @@
       <c r="F15">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -715,8 +904,14 @@
       <c r="F16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -729,8 +924,14 @@
       <c r="F17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G17" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -743,8 +944,14 @@
       <c r="F18">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -757,8 +964,14 @@
       <c r="F19">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -771,8 +984,14 @@
       <c r="F20">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G20" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -785,8 +1004,14 @@
       <c r="F21">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -799,8 +1024,14 @@
       <c r="F22">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -813,8 +1044,14 @@
       <c r="F23">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -827,8 +1064,14 @@
       <c r="F24">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -841,8 +1084,14 @@
       <c r="F25">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G25" t="s">
+        <v>79</v>
+      </c>
+      <c r="I25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -855,8 +1104,14 @@
       <c r="F26">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -869,8 +1124,14 @@
       <c r="F27">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I27">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -883,8 +1144,14 @@
       <c r="F28">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G28" t="s">
+        <v>75</v>
+      </c>
+      <c r="I28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -897,8 +1164,14 @@
       <c r="F29">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G29" t="s">
+        <v>76</v>
+      </c>
+      <c r="I29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -910,6 +1183,124 @@
       </c>
       <c r="F30">
         <v>30</v>
+      </c>
+      <c r="G30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G31" t="s">
+        <v>68</v>
+      </c>
+      <c r="I31">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G32" t="s">
+        <v>69</v>
+      </c>
+      <c r="I32">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G33" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G34" t="s">
+        <v>70</v>
+      </c>
+      <c r="I34">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G35" t="s">
+        <v>71</v>
+      </c>
+      <c r="I35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G36" t="s">
+        <v>65</v>
+      </c>
+      <c r="I36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G37" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G38" t="s">
+        <v>80</v>
+      </c>
+      <c r="I38">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G39" t="s">
+        <v>55</v>
+      </c>
+      <c r="I39">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G40" t="s">
+        <v>77</v>
+      </c>
+      <c r="I40">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G41" t="s">
+        <v>78</v>
+      </c>
+      <c r="I41">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G42" t="s">
+        <v>78</v>
+      </c>
+      <c r="I42">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G43" t="s">
+        <v>78</v>
+      </c>
+      <c r="I43">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="7:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G44" t="s">
+        <v>64</v>
+      </c>
+      <c r="I44">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>